<commit_message>
总结最优效率。gts250 +530%、gtx670 +1800% 。 gts250 最优        GPU --aligned=1 --separate=1 --sort=1 --memory=1 相对  - 67%   +400%        + 3%       -43%     +560% 绝对  - 67%   + 60%        +67%       - 4%     +530%
gts250 第二优
       GPU --aligned=1 --separate=1 --sort=2 --memory=1
相对   -67%   +400%        + 3%       + 4%     + 84%
绝对   -67%   + 60%        +67%       +74%     +220%

gtx670 最优
       GPU --aligned=1 --separate=0 --sort=1 --memory=0
相对  +230%   +120%       +  0%     + 150%     +   0%
绝对  +230%   +660%       +660%     +1800%     +1800%

gtx670 第二优
       GPU --aligned=1 --separate=1 --sort=1 --memory=0
相对  +230%   +120%       + 30%     +  87%     +   0%
绝对  +230%   +660%       +900%     +1750%     +1750%

gtx670 第三优
       GPU --aligned=1 --separate=2 --sort=1 --memory=0
相对  +230%   +120%      +  64%     +  36%     +   0%
绝对  +230%   +660%      +1100%     +1600%     +1600%
</commit_message>
<xml_diff>
--- a/doc/基于CUDA的三维动画实时绘制效率改善算法.xlsx
+++ b/doc/基于CUDA的三维动画实时绘制效率改善算法.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="7500" windowHeight="5220" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="7500" windowHeight="5220" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.问题规模与时间效率的关系-CPU单线程" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="9.问题规模与时间效率的关系-节约" sheetId="12" r:id="rId9"/>
     <sheet name="10.VisualProfiler&amp;OccupancyCalc" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="283">
   <si>
     <t>表1.1</t>
   </si>
@@ -1108,20 +1108,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>交叉时，常量
-优于非常量</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>？</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>参照 最优</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>最优</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1145,15 +1132,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>-67% 相对</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>+120% 相对</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>+400% 相对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1161,23 +1140,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>+7% 相对</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>顺序排序</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>+260% 相对</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>常量最优</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>-12% 相对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1197,15 +1160,28 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>+1800% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>交叉拆分常量
+优于非常量</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+400% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>+60% 绝对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>+1800% 绝对</t>
+    <t>-67% 相对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>+70% 绝对</t>
+    <t>+260% 相对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1213,7 +1189,103 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>+1500% 绝对</t>
+    <t>拆分最优</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>排序最优</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+3% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+67% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+74% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+4% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>排序</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-43% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-4% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+560% 相对非常量</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+84% 相对非常量</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+220% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+30% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+900% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+64% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1100% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1600%</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">+36% </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">+87% </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1750%</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1600% 绝对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-2% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-33% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-23% 相对</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1340% 绝对</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1397,7 +1469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1568,6 +1640,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1583,16 +1668,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1744,11 +1819,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="153180416"/>
-        <c:axId val="153190784"/>
+        <c:axId val="118731136"/>
+        <c:axId val="118733056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="153180416"/>
+        <c:axId val="118731136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,17 +1844,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153190784"/>
+        <c:crossAx val="118733056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153190784"/>
+        <c:axId val="118733056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,25 +1875,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153180416"/>
+        <c:crossAx val="118731136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1925,7 +1997,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.5914376024249033E-2"/>
-                  <c:y val="9.1944643283226074E-2"/>
+                  <c:y val="9.1944643283226116E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1936,7 +2008,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.5914376024249012E-2"/>
-                  <c:y val="0.10204565338423614"/>
+                  <c:y val="0.10204565338423617"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1947,7 +2019,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.5914376024249033E-2"/>
-                  <c:y val="0.11214666348524616"/>
+                  <c:y val="0.11214666348524618"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1958,7 +2030,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.5914376024249033E-2"/>
-                  <c:y val="0.1121466634852462"/>
+                  <c:y val="0.11214666348524623"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1968,8 +2040,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.5914376024248978E-2"/>
-                  <c:y val="0.1020456533842361"/>
+                  <c:x val="-4.5914376024248998E-2"/>
+                  <c:y val="0.10204565338423613"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1980,7 +2052,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.5914376024249033E-2"/>
-                  <c:y val="0.12224767358625635"/>
+                  <c:y val="0.12224767358625642"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -2108,11 +2180,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166251520"/>
-        <c:axId val="166290560"/>
+        <c:axId val="120833152"/>
+        <c:axId val="120835072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166251520"/>
+        <c:axId val="120833152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,14 +2208,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166290560"/>
+        <c:crossAx val="120835072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166290560"/>
+        <c:axId val="120835072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2169,7 +2241,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166251520"/>
+        <c:crossAx val="120833152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2183,7 +2255,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2355,25 +2427,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>125</c:v>
+                  <c:v>113.63636363636364</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>138.88888888888889</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>156.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>178.57142857142856</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>185.18518518518516</c:v>
+                  <c:v>158.73015873015873</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>194.17475728155341</c:v>
+                  <c:v>156.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>201.00502512562812</c:v>
+                  <c:v>158.102766798419</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>205.65552699228792</c:v>
+                  <c:v>158.41584158415841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2383,11 +2455,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166313344"/>
-        <c:axId val="166327808"/>
+        <c:axId val="121951744"/>
+        <c:axId val="121953664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166313344"/>
+        <c:axId val="121951744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2411,14 +2483,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166327808"/>
+        <c:crossAx val="121953664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166327808"/>
+        <c:axId val="121953664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2516,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166313344"/>
+        <c:crossAx val="121951744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2458,7 +2530,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2646,11 +2718,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166370688"/>
-        <c:axId val="166385152"/>
+        <c:axId val="122004992"/>
+        <c:axId val="122006912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166370688"/>
+        <c:axId val="122004992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2674,14 +2746,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166385152"/>
+        <c:crossAx val="122006912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166385152"/>
+        <c:axId val="122006912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,7 +2779,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166370688"/>
+        <c:crossAx val="122004992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2721,7 +2793,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2922,11 +2994,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166559744"/>
-        <c:axId val="166561664"/>
+        <c:axId val="127371136"/>
+        <c:axId val="127377408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166559744"/>
+        <c:axId val="127371136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,14 +3022,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166561664"/>
+        <c:crossAx val="127377408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166561664"/>
+        <c:axId val="127377408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2983,7 +3055,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166559744"/>
+        <c:crossAx val="127371136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2997,7 +3069,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3197,11 +3269,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166621568"/>
-        <c:axId val="166623488"/>
+        <c:axId val="127420672"/>
+        <c:axId val="127426944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166621568"/>
+        <c:axId val="127420672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,14 +3297,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166623488"/>
+        <c:crossAx val="127426944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166623488"/>
+        <c:axId val="127426944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3330,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166621568"/>
+        <c:crossAx val="127420672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3272,7 +3344,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3545,9 +3617,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$L$17:$L$23</c:f>
@@ -3643,9 +3712,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$N$17:$N$23</c:f>
@@ -3692,9 +3758,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$O$17:$O$23</c:f>
@@ -3730,11 +3793,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166671872"/>
-        <c:axId val="166673792"/>
+        <c:axId val="127602048"/>
+        <c:axId val="127645184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166671872"/>
+        <c:axId val="127602048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3765,7 +3828,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3809,14 +3871,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166673792"/>
+        <c:crossAx val="127645184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166673792"/>
+        <c:axId val="127645184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3861,7 +3923,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3900,7 +3961,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166671872"/>
+        <c:crossAx val="127602048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3914,7 +3975,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3973,7 +4033,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4246,9 +4306,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$L$4:$L$10</c:f>
@@ -4295,9 +4352,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$M$4:$M$10</c:f>
@@ -4344,9 +4398,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$N$4:$N$10</c:f>
@@ -4432,11 +4483,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="172918272"/>
-        <c:axId val="172920192"/>
+        <c:axId val="127716736"/>
+        <c:axId val="128013824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172918272"/>
+        <c:axId val="127716736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4467,7 +4518,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4511,14 +4561,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172920192"/>
+        <c:crossAx val="128013824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172920192"/>
+        <c:axId val="128013824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4563,7 +4613,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4602,7 +4651,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172918272"/>
+        <c:crossAx val="127716736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4616,7 +4665,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4675,7 +4723,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4813,11 +4861,11 @@
         </c:dLbls>
         <c:dropLines/>
         <c:marker val="1"/>
-        <c:axId val="172952960"/>
-        <c:axId val="172955136"/>
+        <c:axId val="128050688"/>
+        <c:axId val="128052608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172952960"/>
+        <c:axId val="128050688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4854,14 +4902,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172955136"/>
+        <c:crossAx val="128052608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172955136"/>
+        <c:axId val="128052608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4892,7 +4940,7 @@
         </c:title>
         <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172952960"/>
+        <c:crossAx val="128050688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4906,7 +4954,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5229,9 +5277,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$M$59:$M$65</c:f>
@@ -5327,9 +5372,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$O$59:$O$65</c:f>
@@ -5365,11 +5407,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="173052288"/>
-        <c:axId val="173054208"/>
+        <c:axId val="128203008"/>
+        <c:axId val="128221568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173052288"/>
+        <c:axId val="128203008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5400,7 +5442,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -5444,14 +5485,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173054208"/>
+        <c:crossAx val="128221568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173054208"/>
+        <c:axId val="128221568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5496,7 +5537,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -5535,7 +5575,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173052288"/>
+        <c:crossAx val="128203008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5549,7 +5589,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5608,7 +5647,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5881,9 +5920,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$L$86:$L$92</c:f>
@@ -5930,9 +5966,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$M$86:$M$92</c:f>
@@ -5979,9 +6012,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$N$86:$N$92</c:f>
@@ -6028,9 +6058,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$O$86:$O$92</c:f>
@@ -6066,11 +6093,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="173134208"/>
-        <c:axId val="173136128"/>
+        <c:axId val="128297216"/>
+        <c:axId val="128307584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173134208"/>
+        <c:axId val="128297216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6101,6 +6128,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -6144,14 +6172,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173136128"/>
+        <c:crossAx val="128307584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173136128"/>
+        <c:axId val="128307584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6196,6 +6224,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -6234,7 +6263,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173134208"/>
+        <c:crossAx val="128297216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6248,6 +6277,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6306,7 +6336,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6446,11 +6476,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="159655424"/>
-        <c:axId val="159657344"/>
+        <c:axId val="118963584"/>
+        <c:axId val="118990336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159655424"/>
+        <c:axId val="118963584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6471,17 +6501,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159657344"/>
+        <c:crossAx val="118990336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159657344"/>
+        <c:axId val="118990336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6503,25 +6532,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159655424"/>
+        <c:crossAx val="118963584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6794,9 +6821,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$L$72:$L$78</c:f>
@@ -6843,9 +6867,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$M$72:$M$78</c:f>
@@ -6892,9 +6913,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$N$72:$N$78</c:f>
@@ -6941,9 +6959,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$O$72:$O$78</c:f>
@@ -6979,11 +6994,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="172876160"/>
-        <c:axId val="172878080"/>
+        <c:axId val="128383232"/>
+        <c:axId val="128532864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172876160"/>
+        <c:axId val="128383232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7058,14 +7073,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172878080"/>
+        <c:crossAx val="128532864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172878080"/>
+        <c:axId val="128532864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7149,7 +7164,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172876160"/>
+        <c:crossAx val="128383232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7222,7 +7237,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7446,9 +7461,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'6.问题规模与时间效率的关系-常量'!$L$45:$L$51</c:f>
@@ -7514,7 +7526,7 @@
                   <c:v>172.41379310344828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>188.67924528301884</c:v>
+                  <c:v>185.18518518518516</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>194.17475728155341</c:v>
@@ -7612,7 +7624,7 @@
                   <c:v>166.66666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175.43859649122808</c:v>
+                  <c:v>169.49152542372883</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>180.18018018018017</c:v>
@@ -7631,11 +7643,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="114647424"/>
-        <c:axId val="114649344"/>
+        <c:axId val="128606976"/>
+        <c:axId val="128608896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114647424"/>
+        <c:axId val="128606976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7666,7 +7678,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -7710,14 +7721,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114649344"/>
+        <c:crossAx val="128608896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114649344"/>
+        <c:axId val="128608896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7762,7 +7773,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -7801,7 +7811,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114647424"/>
+        <c:crossAx val="128606976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7815,7 +7825,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7874,7 +7883,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8134,11 +8143,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="114798592"/>
-        <c:axId val="114800512"/>
+        <c:axId val="128995712"/>
+        <c:axId val="128997632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114798592"/>
+        <c:axId val="128995712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8169,7 +8178,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8213,14 +8221,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114800512"/>
+        <c:crossAx val="128997632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114800512"/>
+        <c:axId val="128997632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8265,7 +8273,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8304,7 +8311,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114798592"/>
+        <c:crossAx val="128995712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8318,7 +8325,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -8377,7 +8383,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8637,11 +8643,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="152656896"/>
-        <c:axId val="152679552"/>
+        <c:axId val="129019264"/>
+        <c:axId val="129119744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152656896"/>
+        <c:axId val="129019264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8672,7 +8678,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8716,14 +8721,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152679552"/>
+        <c:crossAx val="129119744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152679552"/>
+        <c:axId val="129119744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8768,7 +8773,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8807,7 +8811,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152656896"/>
+        <c:crossAx val="129019264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8821,7 +8825,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -8880,7 +8883,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9078,24 +9081,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114886912"/>
-        <c:axId val="114913280"/>
+        <c:axId val="129174144"/>
+        <c:axId val="129192320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114886912"/>
+        <c:axId val="129174144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114913280"/>
+        <c:crossAx val="129192320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114913280"/>
+        <c:axId val="129192320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9103,7 +9106,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114886912"/>
+        <c:crossAx val="129174144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9116,7 +9119,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9298,24 +9301,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114939392"/>
-        <c:axId val="114940928"/>
+        <c:axId val="129349504"/>
+        <c:axId val="129351040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114939392"/>
+        <c:axId val="129349504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114940928"/>
+        <c:crossAx val="129351040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114940928"/>
+        <c:axId val="129351040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9323,7 +9326,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114939392"/>
+        <c:crossAx val="129349504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9336,7 +9339,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9526,11 +9529,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="114979584"/>
-        <c:axId val="114981120"/>
+        <c:axId val="129406080"/>
+        <c:axId val="129407616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114979584"/>
+        <c:axId val="129406080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9542,14 +9545,14 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114981120"/>
+        <c:crossAx val="129407616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114981120"/>
+        <c:axId val="129407616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9557,7 +9560,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114979584"/>
+        <c:crossAx val="129406080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9570,7 +9573,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9892,11 +9895,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115181440"/>
-        <c:axId val="115200000"/>
+        <c:axId val="131442944"/>
+        <c:axId val="131453312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115181440"/>
+        <c:axId val="131442944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9970,14 +9973,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115200000"/>
+        <c:crossAx val="131453312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115200000"/>
+        <c:axId val="131453312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10060,7 +10063,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115181440"/>
+        <c:crossAx val="131442944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10132,7 +10135,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10381,7 +10384,7 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.8246072431043199E-17"/>
+                  <c:x val="-8.8246072431043421E-17"/>
                   <c:y val="0.11666666666666672"/>
                 </c:manualLayout>
               </c:layout>
@@ -10520,7 +10523,7 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.6474127557160252E-2"/>
+                  <c:x val="-2.6474127557160262E-2"/>
                   <c:y val="-5.0000000000000024E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -10533,7 +10536,7 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.4067388688327449E-2"/>
+                  <c:x val="-2.406738868832746E-2"/>
                   <c:y val="-7.2222222222222424E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -10643,11 +10646,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115116288"/>
-        <c:axId val="115143040"/>
+        <c:axId val="138275456"/>
+        <c:axId val="138420992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115116288"/>
+        <c:axId val="138275456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10721,14 +10724,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115143040"/>
+        <c:crossAx val="138420992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115143040"/>
+        <c:axId val="138420992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10811,7 +10814,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115116288"/>
+        <c:crossAx val="138275456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10883,7 +10886,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11143,11 +11146,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115275648"/>
-        <c:axId val="115294208"/>
+        <c:axId val="138512640"/>
+        <c:axId val="138514816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115275648"/>
+        <c:axId val="138512640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11221,14 +11224,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115294208"/>
+        <c:crossAx val="138514816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115294208"/>
+        <c:axId val="138514816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11311,7 +11314,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115275648"/>
+        <c:crossAx val="138512640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11383,7 +11386,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11523,11 +11526,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="159732864"/>
-        <c:axId val="159734784"/>
+        <c:axId val="120269824"/>
+        <c:axId val="120280192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159732864"/>
+        <c:axId val="120269824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11551,14 +11554,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159734784"/>
+        <c:crossAx val="120280192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159734784"/>
+        <c:axId val="120280192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11584,7 +11587,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159732864"/>
+        <c:crossAx val="120269824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11598,7 +11601,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11858,11 +11861,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115328128"/>
-        <c:axId val="115330048"/>
+        <c:axId val="138573312"/>
+        <c:axId val="138575232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115328128"/>
+        <c:axId val="138573312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11936,14 +11939,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115330048"/>
+        <c:crossAx val="138575232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115330048"/>
+        <c:axId val="138575232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12026,7 +12029,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115328128"/>
+        <c:crossAx val="138573312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12098,7 +12101,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12418,11 +12421,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115394048"/>
-        <c:axId val="115395968"/>
+        <c:axId val="138700672"/>
+        <c:axId val="138715136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115394048"/>
+        <c:axId val="138700672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12496,14 +12499,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115395968"/>
+        <c:crossAx val="138715136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115395968"/>
+        <c:axId val="138715136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12586,7 +12589,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115394048"/>
+        <c:crossAx val="138700672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12658,7 +12661,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12978,11 +12981,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115451776"/>
-        <c:axId val="115478528"/>
+        <c:axId val="139032832"/>
+        <c:axId val="139051392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115451776"/>
+        <c:axId val="139032832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13056,14 +13059,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115478528"/>
+        <c:crossAx val="139051392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115478528"/>
+        <c:axId val="139051392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13146,7 +13149,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115451776"/>
+        <c:crossAx val="139032832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13218,7 +13221,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13361,25 +13364,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115556736"/>
-        <c:axId val="115558272"/>
+        <c:axId val="140256000"/>
+        <c:axId val="140257536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115556736"/>
+        <c:axId val="140256000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115558272"/>
+        <c:crossAx val="140257536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115558272"/>
+        <c:axId val="140257536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13388,7 +13391,7 @@
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115556736"/>
+        <c:crossAx val="140256000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13401,7 +13404,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13544,25 +13547,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115587712"/>
-        <c:axId val="115597696"/>
+        <c:axId val="140278784"/>
+        <c:axId val="140305152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115587712"/>
+        <c:axId val="140278784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115597696"/>
+        <c:crossAx val="140305152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115597696"/>
+        <c:axId val="140305152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13570,7 +13573,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115587712"/>
+        <c:crossAx val="140278784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13583,7 +13586,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13726,25 +13729,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115623040"/>
-        <c:axId val="115624576"/>
+        <c:axId val="140334592"/>
+        <c:axId val="140336128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115623040"/>
+        <c:axId val="140334592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115624576"/>
+        <c:crossAx val="140336128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115624576"/>
+        <c:axId val="140336128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13752,7 +13755,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115623040"/>
+        <c:crossAx val="140334592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13765,7 +13768,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13908,25 +13911,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="115662208"/>
-        <c:axId val="115672192"/>
+        <c:axId val="140464128"/>
+        <c:axId val="140465664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115662208"/>
+        <c:axId val="140464128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115672192"/>
+        <c:crossAx val="140465664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115672192"/>
+        <c:axId val="140465664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13934,7 +13937,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115662208"/>
+        <c:crossAx val="140464128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13947,7 +13950,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14087,11 +14090,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="163991936"/>
-        <c:axId val="163993856"/>
+        <c:axId val="120318208"/>
+        <c:axId val="120328576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163991936"/>
+        <c:axId val="120318208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14115,14 +14118,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163993856"/>
+        <c:crossAx val="120328576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163993856"/>
+        <c:axId val="120328576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14148,7 +14151,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163991936"/>
+        <c:crossAx val="120318208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14162,7 +14165,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14302,11 +14305,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="164118528"/>
-        <c:axId val="164120448"/>
+        <c:axId val="120485760"/>
+        <c:axId val="120492032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="164118528"/>
+        <c:axId val="120485760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14330,14 +14333,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164120448"/>
+        <c:crossAx val="120492032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164120448"/>
+        <c:axId val="120492032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14363,7 +14366,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164118528"/>
+        <c:crossAx val="120485760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14377,7 +14380,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14517,11 +14520,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="164133888"/>
-        <c:axId val="164164736"/>
+        <c:axId val="120509568"/>
+        <c:axId val="120511488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="164133888"/>
+        <c:axId val="120509568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14545,14 +14548,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164164736"/>
+        <c:crossAx val="120511488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164164736"/>
+        <c:axId val="120511488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14578,7 +14581,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164133888"/>
+        <c:crossAx val="120509568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14592,7 +14595,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14732,11 +14735,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166148736"/>
-        <c:axId val="166159104"/>
+        <c:axId val="120566528"/>
+        <c:axId val="120568448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166148736"/>
+        <c:axId val="120566528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14760,14 +14763,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166159104"/>
+        <c:crossAx val="120568448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166159104"/>
+        <c:axId val="120568448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14793,7 +14796,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166148736"/>
+        <c:crossAx val="120566528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14807,7 +14810,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14947,11 +14950,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166184832"/>
-        <c:axId val="166076416"/>
+        <c:axId val="120619008"/>
+        <c:axId val="120620928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166184832"/>
+        <c:axId val="120619008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14975,14 +14978,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166076416"/>
+        <c:crossAx val="120620928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166076416"/>
+        <c:axId val="120620928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15008,7 +15011,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166184832"/>
+        <c:crossAx val="120619008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15022,7 +15025,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -15222,11 +15225,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="166210176"/>
-        <c:axId val="166224640"/>
+        <c:axId val="120804096"/>
+        <c:axId val="120806016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166210176"/>
+        <c:axId val="120804096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15250,14 +15253,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166224640"/>
+        <c:crossAx val="120806016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166224640"/>
+        <c:axId val="120806016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15283,7 +15286,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166210176"/>
+        <c:crossAx val="120804096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15297,7 +15300,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -17227,26 +17230,26 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="102.75" customHeight="1">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
     </row>
     <row r="31" spans="1:14" ht="48.75" customHeight="1">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -18172,8 +18175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18421,8 +18424,8 @@
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="E12" s="68" t="s">
-        <v>244</v>
+      <c r="E12" s="63" t="s">
+        <v>241</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>25</v>
@@ -18436,7 +18439,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="E13" s="59" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -18678,8 +18681,8 @@
       <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="E26" s="68" t="s">
-        <v>245</v>
+      <c r="E26" s="63" t="s">
+        <v>242</v>
       </c>
       <c r="L26" s="20" t="s">
         <v>28</v>
@@ -18693,20 +18696,20 @@
     </row>
     <row r="27" spans="1:14">
       <c r="E27" s="59" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="116.25" customHeight="1">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="7"/>
@@ -18822,7 +18825,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19069,8 +19072,8 @@
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="E12" s="68" t="s">
-        <v>246</v>
+      <c r="E12" s="63" t="s">
+        <v>243</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>36</v>
@@ -19083,8 +19086,8 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="E13" s="68" t="s">
-        <v>257</v>
+      <c r="E13" s="63" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="54">
@@ -19316,7 +19319,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="24"/>
       <c r="F25" s="59" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G25" s="23"/>
       <c r="L25" s="10" t="s">
@@ -19330,38 +19333,38 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="E26" s="68" t="s">
-        <v>247</v>
+      <c r="E26" s="63" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="E27" s="68" t="s">
-        <v>258</v>
+      <c r="E27" s="63" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="136.5" customHeight="1">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
     </row>
     <row r="31" spans="1:14" ht="39" customHeight="1">
-      <c r="A31" s="62" t="s">
+      <c r="A31" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19379,8 +19382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:H28"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19628,8 +19631,8 @@
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="E12" s="68" t="s">
-        <v>248</v>
+      <c r="E12" s="63" t="s">
+        <v>244</v>
       </c>
       <c r="L12" t="s">
         <v>51</v>
@@ -19642,8 +19645,8 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="E13" s="68" t="s">
-        <v>259</v>
+      <c r="E13" s="63" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="40.5">
@@ -19886,26 +19889,26 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="E26" s="68" t="s">
-        <v>249</v>
+      <c r="E26" s="63" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="E27" s="68" t="s">
-        <v>260</v>
+      <c r="E27" s="63" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="148.5" customHeight="1">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19921,8 +19924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20107,8 +20110,8 @@
       <c r="G7" s="49">
         <v>6.16</v>
       </c>
-      <c r="H7" s="8">
-        <f t="shared" si="3"/>
+      <c r="H7" s="58">
+        <f>B7/I7*50</f>
         <v>16.694490818030051</v>
       </c>
       <c r="I7" s="4">
@@ -20216,7 +20219,10 @@
     </row>
     <row r="11" spans="1:13">
       <c r="F11" s="59" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>258</v>
       </c>
       <c r="K11" t="s">
         <v>66</v>
@@ -20226,6 +20232,16 @@
       </c>
       <c r="M11" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="H12" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="H13" s="63" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="40.5">
@@ -20387,8 +20403,8 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="E20" s="8">
-        <f t="shared" si="5"/>
+      <c r="E20" s="58">
+        <f>B20/C20*50</f>
         <v>125</v>
       </c>
       <c r="F20" s="58">
@@ -20398,7 +20414,7 @@
       <c r="G20" s="4">
         <v>1.31</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="58">
         <f t="shared" si="7"/>
         <v>99.009900990099013</v>
       </c>
@@ -20519,6 +20535,22 @@
         <v>72</v>
       </c>
     </row>
+    <row r="25" spans="1:13">
+      <c r="E25" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="E26" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="H26" s="63" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="27" spans="1:13" ht="27">
       <c r="C27" s="10" t="s">
         <v>73</v>
@@ -20527,7 +20559,7 @@
         <v>54</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F27" s="35" t="s">
         <v>74</v>
@@ -20699,7 +20731,7 @@
       <c r="G33" s="49">
         <v>8.89</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="58">
         <f t="shared" si="11"/>
         <v>9.5785440613026829</v>
       </c>
@@ -20815,6 +20847,9 @@
       <c r="K36" s="17"/>
     </row>
     <row r="37" spans="1:14">
+      <c r="H37" s="59" t="s">
+        <v>264</v>
+      </c>
       <c r="L37" t="s">
         <v>75</v>
       </c>
@@ -20823,6 +20858,16 @@
       </c>
       <c r="N37" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="H38" s="63" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="H39" s="63" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="27">
@@ -20833,7 +20878,7 @@
         <v>70</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F40" s="35" t="s">
         <v>74</v>
@@ -20986,7 +21031,7 @@
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="58">
         <f t="shared" si="13"/>
         <v>169.49152542372883</v>
       </c>
@@ -20997,7 +21042,7 @@
       <c r="G46" s="4">
         <v>0.53</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="58">
         <f t="shared" si="15"/>
         <v>185.18518518518516</v>
       </c>
@@ -21119,13 +21164,25 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="F51" s="68" t="s">
-        <v>250</v>
+      <c r="E51" s="63" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="H51" s="63" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="F52" s="68" t="s">
-        <v>261</v>
+      <c r="E52" s="63" t="s">
+        <v>274</v>
+      </c>
+      <c r="F52" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="H52" s="63" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="27">
@@ -21203,10 +21260,10 @@
       </c>
       <c r="H56" s="8">
         <f>B56/I56*50</f>
-        <v>125</v>
+        <v>113.63636363636364</v>
       </c>
       <c r="I56" s="4">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -21236,10 +21293,10 @@
       </c>
       <c r="H57" s="8">
         <f t="shared" ref="H57:H62" si="19">B57/I57*50</f>
-        <v>156.25</v>
+        <v>138.88888888888889</v>
       </c>
       <c r="I57" s="4">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -21269,10 +21326,10 @@
       </c>
       <c r="H58" s="8">
         <f t="shared" si="19"/>
-        <v>178.57142857142856</v>
+        <v>156.25</v>
       </c>
       <c r="I58" s="42">
-        <v>0.28000000000000003</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -21302,10 +21359,10 @@
       </c>
       <c r="H59" s="8">
         <f t="shared" si="19"/>
-        <v>185.18518518518516</v>
+        <v>158.73015873015873</v>
       </c>
       <c r="I59" s="4">
-        <v>0.54</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -21335,10 +21392,10 @@
       </c>
       <c r="H60" s="8">
         <f t="shared" si="19"/>
-        <v>194.17475728155341</v>
+        <v>156.25</v>
       </c>
       <c r="I60" s="4">
-        <v>1.03</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -21368,10 +21425,10 @@
       </c>
       <c r="H61" s="8">
         <f t="shared" si="19"/>
-        <v>201.00502512562812</v>
+        <v>158.102766798419</v>
       </c>
       <c r="I61" s="4">
-        <v>1.99</v>
+        <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -21401,10 +21458,10 @@
       </c>
       <c r="H62" s="8">
         <f t="shared" si="19"/>
-        <v>205.65552699228792</v>
+        <v>158.41584158415841</v>
       </c>
       <c r="I62" s="4">
-        <v>3.89</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -21699,7 +21756,7 @@
     </row>
     <row r="76" spans="1:14">
       <c r="H76" s="59" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="L76" t="s">
         <v>84</v>
@@ -21712,26 +21769,26 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="H77" s="68" t="s">
-        <v>251</v>
+      <c r="H77" s="63" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="H78" s="68" t="s">
+      <c r="H78" s="63" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="192" customHeight="1">
-      <c r="A79" s="63" t="s">
+      <c r="A79" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="64"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="64"/>
-      <c r="H79" s="64"/>
+      <c r="B79" s="69"/>
+      <c r="C79" s="69"/>
+      <c r="D79" s="69"/>
+      <c r="E79" s="69"/>
+      <c r="F79" s="69"/>
+      <c r="G79" s="69"/>
+      <c r="H79" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21746,10 +21803,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V93"/>
+  <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -22922,16 +22979,16 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="173.25" customHeight="1">
-      <c r="A38" s="60" t="s">
+      <c r="A38" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
     </row>
     <row r="42" spans="1:15" ht="40.5">
       <c r="C42" s="10" t="s">
@@ -23175,7 +23232,7 @@
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="58">
         <f t="shared" si="16"/>
         <v>144.92753623188409</v>
       </c>
@@ -23183,36 +23240,36 @@
         <f t="shared" si="18"/>
         <v>188.67924528301884</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="64">
         <v>0.53</v>
       </c>
       <c r="H48" s="4">
         <v>0.81</v>
       </c>
       <c r="I48" s="4">
-        <v>0.53</v>
-      </c>
-      <c r="J48" s="4">
+        <v>0.54</v>
+      </c>
+      <c r="J48" s="64">
         <v>0.6</v>
       </c>
       <c r="K48" s="4">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L48" s="8">
-        <f t="shared" si="19"/>
+        <v>0.59</v>
+      </c>
+      <c r="L48" s="58">
+        <f>B48/H48*50</f>
         <v>123.45679012345678</v>
       </c>
-      <c r="M48" s="8">
+      <c r="M48" s="58">
         <f t="shared" si="20"/>
-        <v>188.67924528301884</v>
+        <v>185.18518518518516</v>
       </c>
       <c r="N48" s="58">
         <f t="shared" si="21"/>
         <v>166.66666666666669</v>
       </c>
-      <c r="O48" s="8">
+      <c r="O48" s="58">
         <f t="shared" si="22"/>
-        <v>175.43859649122808</v>
+        <v>169.49152542372883</v>
       </c>
     </row>
     <row r="49" spans="1:22">
@@ -23382,16 +23439,13 @@
       <c r="B52" s="16"/>
       <c r="C52" s="17"/>
       <c r="D52" s="16"/>
-      <c r="E52" s="65" t="s">
+      <c r="E52" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F52" s="18"/>
-      <c r="G52" s="67" t="s">
-        <v>240</v>
-      </c>
-      <c r="N52" s="59" t="s">
-        <v>254</v>
-      </c>
+      <c r="F52" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="N52" s="59"/>
       <c r="U52" t="s">
         <v>222</v>
       </c>
@@ -23400,13 +23454,25 @@
       </c>
     </row>
     <row r="53" spans="1:22">
-      <c r="N53" s="68" t="s">
-        <v>255</v>
+      <c r="E53" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="L53" s="63" t="s">
+        <v>280</v>
+      </c>
+      <c r="N53" s="63" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:22">
-      <c r="N54" s="68" t="s">
-        <v>264</v>
+      <c r="E54" s="63" t="s">
+        <v>282</v>
+      </c>
+      <c r="L54" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="N54" s="63" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:22" ht="40.5">
@@ -23665,7 +23731,7 @@
       <c r="G62" s="4">
         <v>8.8699999999999992</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="64">
         <v>1.58</v>
       </c>
       <c r="I62" s="4">
@@ -23868,13 +23934,19 @@
       </c>
     </row>
     <row r="67" spans="1:22">
-      <c r="L67" s="68" t="s">
-        <v>253</v>
+      <c r="L67" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="N67" s="63" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:22">
-      <c r="L68" s="68" t="s">
-        <v>263</v>
+      <c r="L68" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="N68" s="63" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:22" ht="40.5">
@@ -23891,7 +23963,7 @@
         <v>217</v>
       </c>
       <c r="G69" s="25"/>
-      <c r="H69" s="66" t="s">
+      <c r="H69" s="61" t="s">
         <v>237</v>
       </c>
     </row>
@@ -24353,12 +24425,10 @@
         <v>217</v>
       </c>
       <c r="G83" s="7"/>
-      <c r="H83" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="I83" s="10" t="s">
-        <v>239</v>
-      </c>
+      <c r="H83" s="61" t="s">
+        <v>252</v>
+      </c>
+      <c r="I83" s="10"/>
     </row>
     <row r="84" spans="1:22">
       <c r="F84" s="7"/>
@@ -24610,7 +24680,7 @@
       <c r="K89" s="4">
         <v>15.77</v>
       </c>
-      <c r="L89" s="8">
+      <c r="L89" s="58">
         <f t="shared" si="40"/>
         <v>32.051282051282051</v>
       </c>
@@ -24798,6 +24868,16 @@
       </c>
       <c r="V93" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22">
+      <c r="L94" s="63" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22">
+      <c r="L95" s="63" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -24815,7 +24895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -25307,16 +25387,16 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="212.25" customHeight="1">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
     </row>
     <row r="32" spans="1:15" ht="40.5">
       <c r="C32" s="10" t="s">
@@ -28059,16 +28139,16 @@
       <c r="G28" s="51"/>
     </row>
     <row r="29" spans="1:15" ht="194.25" customHeight="1">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28670,16 +28750,16 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="96.75" customHeight="1">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="65" t="s">
         <v>164</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
     </row>
     <row r="32" spans="1:14" ht="40.5">
       <c r="C32" s="10" t="s">

</xml_diff>